<commit_message>
edits to resetting treatment variables
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_PregnancySupervisor.xlsx
+++ b/resources/ResourceFile_PregnancySupervisor.xlsx
@@ -9,14 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11676" windowHeight="6216" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11670" windowHeight="6210"/>
   </bookViews>
   <sheets>
     <sheet name="parameter_values" sheetId="1" r:id="rId1"/>
-    <sheet name="prob_pregnancy_factors" sheetId="2" r:id="rId2"/>
-    <sheet name="prob_maternal_death" sheetId="5" r:id="rId3"/>
-    <sheet name="md calculation" sheetId="3" r:id="rId4"/>
-    <sheet name="prob_stillbirth" sheetId="4" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId2"/>
+    <sheet name="prob_pregnancy_factors" sheetId="2" r:id="rId3"/>
+    <sheet name="prob_maternal_death" sheetId="5" r:id="rId4"/>
+    <sheet name="md calculation" sheetId="3" r:id="rId5"/>
+    <sheet name="prob_stillbirth" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -62,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="94">
   <si>
     <t>parameter_name</t>
   </si>
@@ -142,37 +143,6 @@
     <t>rr_gest_diab_chron_htn</t>
   </si>
   <si>
-    <t>base_prev_pe</t>
-  </si>
-  <si>
-    <t>base_prev_gest_htn</t>
-  </si>
-  <si>
-    <t>Pre-eclampsia, eclampsia and adverse maternal and perinatal outcomes: a secondary analysis of the World Health Organization Multicountry Survey on Maternal and Newborn Health.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#DUMMY </t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve"># partially dummy informed by </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Gestational diabetes mellitus in sub-Saharan Africa: Systematic review and metaregression on prevalence and risk factors</t>
-    </r>
-  </si>
-  <si>
-    <t>base_prev_gest_diab</t>
-  </si>
-  <si>
     <t>r_severe_pe_mild_pe</t>
   </si>
   <si>
@@ -354,6 +324,27 @@
   </si>
   <si>
     <t>risk_d_ectopic</t>
+  </si>
+  <si>
+    <t>prob_miscarriage_per_month</t>
+  </si>
+  <si>
+    <t>prob_abortion_per_month</t>
+  </si>
+  <si>
+    <t>prob_pre_eclampsia_per_month</t>
+  </si>
+  <si>
+    <t>prob_gest_htn_per_month</t>
+  </si>
+  <si>
+    <t>prob_gest_diab_per_month</t>
+  </si>
+  <si>
+    <t>prob_still_birth_per_month</t>
+  </si>
+  <si>
+    <t>prob_antenatal_death_per_month</t>
   </si>
 </sst>
 </file>
@@ -763,19 +754,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -786,245 +777,106 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="B2">
-        <v>2.1600000000000001E-2</v>
+        <v>0.02</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="B3">
         <v>0.02</v>
       </c>
-      <c r="E3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>87</v>
       </c>
       <c r="B4">
-        <v>0.05</v>
-      </c>
-      <c r="E4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0.02</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>88</v>
       </c>
       <c r="B5">
-        <v>2.23</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0.02</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>89</v>
       </c>
       <c r="B6">
-        <v>4.0199999999999996</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0.02</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>90</v>
       </c>
       <c r="B7">
-        <v>2.13</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0.02</v>
+      </c>
+      <c r="D7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="B8">
-        <v>0.49</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0.02</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>92</v>
       </c>
       <c r="B9">
-        <v>2.91</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0.02</v>
+      </c>
+      <c r="D9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>93</v>
       </c>
       <c r="B10">
-        <v>7.19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11">
-        <v>3.51</v>
-      </c>
-      <c r="D11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12">
-        <v>2.92</v>
-      </c>
-      <c r="D12" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13">
-        <v>14.6</v>
-      </c>
-      <c r="D13" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14">
-        <v>2.4900000000000002</v>
-      </c>
-      <c r="D14" t="s">
-        <v>21</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15">
         <v>0.02</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D10" t="s">
         <v>19</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16">
-        <v>0.02</v>
-      </c>
-      <c r="D16" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>40</v>
-      </c>
-      <c r="B17">
-        <v>0.6</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>35</v>
-      </c>
-      <c r="B18">
-        <v>3.4000000000000002E-2</v>
-      </c>
-      <c r="D18" t="s">
-        <v>36</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>32</v>
-      </c>
-      <c r="B19">
-        <v>3.4000000000000002E-2</v>
-      </c>
-      <c r="D19" t="s">
-        <v>36</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>33</v>
-      </c>
-      <c r="B20">
-        <v>3.4000000000000002E-2</v>
-      </c>
-      <c r="D20" t="s">
-        <v>36</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>34</v>
-      </c>
-      <c r="B21">
-        <v>3.4000000000000002E-2</v>
-      </c>
-      <c r="D21" t="s">
-        <v>36</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1035,23 +887,224 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:E18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2">
+        <v>2.23</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3">
+        <v>4.0199999999999996</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>2.13</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>0.49</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6">
+        <v>2.91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7">
+        <v>7.19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8">
+        <v>3.51</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9">
+        <v>2.92</v>
+      </c>
+      <c r="D9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10">
+        <v>14.6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11">
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="D11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14">
+        <v>0.6</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="D16" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="D17" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="D18" t="s">
+        <v>30</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1074,7 +1127,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1097,7 +1150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1120,7 +1173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1143,7 +1196,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1166,7 +1219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1189,7 +1242,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1212,7 +1265,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1235,7 +1288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1258,7 +1311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1281,7 +1334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1304,7 +1357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16">
         <f>SUM(B2:B6)</f>
         <v>0.19</v>
@@ -1316,85 +1369,85 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C1" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D1" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="E1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1404,7 +1457,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O23"/>
   <sheetViews>
@@ -1412,24 +1465,24 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="24.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.77734375" customWidth="1"/>
-    <col min="4" max="4" width="12.88671875" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
     <col min="8" max="8" width="11" customWidth="1"/>
     <col min="10" max="10" width="17" customWidth="1"/>
-    <col min="15" max="15" width="25.33203125" customWidth="1"/>
+    <col min="15" max="15" width="25.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B1" s="16" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C4" s="4">
         <v>2010</v>
@@ -1462,72 +1515,72 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C5">
         <v>484</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="H5">
         <v>451</v>
       </c>
       <c r="I5" s="11" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="J5" s="11" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="K5" s="11" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="L5" s="11" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C6" s="6" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="H6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="9" spans="2:15" ht="43.2" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" ht="60" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D9" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="J9" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="H9" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="I9" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="J9" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C10" s="5">
         <v>0.3</v>
@@ -1536,15 +1589,15 @@
         <v>0.22700000000000001</v>
       </c>
       <c r="H10" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="I10" s="10">
         <v>9.6000000000000002E-2</v>
       </c>
     </row>
-    <row r="11" spans="2:15" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:15" ht="45" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C11" s="5">
         <v>0.4</v>
@@ -1553,21 +1606,21 @@
         <v>0.48599999999999999</v>
       </c>
       <c r="H11" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="I11" s="10">
         <v>2.1000000000000001E-2</v>
       </c>
       <c r="K11" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="O11" s="7" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C12" s="5">
         <v>0.3</v>
@@ -1576,73 +1629,73 @@
         <v>0.28699999999999998</v>
       </c>
       <c r="H12" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="I12" s="10">
         <v>0.245</v>
       </c>
     </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H13" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="I13" s="5">
         <v>0.16</v>
       </c>
     </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C14" s="5">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="H14" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="I14" s="10">
         <v>0.10299999999999999</v>
       </c>
     </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C15" s="5">
         <v>0.08</v>
       </c>
       <c r="H15" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="I15" s="5">
         <v>0.09</v>
       </c>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C16" s="5">
         <v>0.15</v>
       </c>
       <c r="H16" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="I16" s="10">
         <v>0.28599999999999998</v>
       </c>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C17" s="5">
         <v>0.4</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C18" s="5">
         <v>0.09</v>
@@ -1652,39 +1705,39 @@
         <v>1.0009999999999999</v>
       </c>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C19" s="5">
         <v>0.21</v>
       </c>
     </row>
-    <row r="21" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:11" ht="45" x14ac:dyDescent="0.25">
       <c r="H21" s="13" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="I21" s="14" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="J21" s="15"/>
       <c r="K21" s="15"/>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
       <c r="H22" s="15"/>
       <c r="I22" s="15" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="J22" s="15" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="K22" s="15" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
       <c r="H23" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="I23" s="5"/>
       <c r="J23" s="5">
@@ -1697,7 +1750,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N18"/>
   <sheetViews>
@@ -1705,20 +1758,20 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B1" s="16" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C4" s="17">
         <v>2010</v>
@@ -1751,164 +1804,164 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="H5">
         <v>21.8</v>
       </c>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="H6" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="8" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" ht="30" x14ac:dyDescent="0.25">
       <c r="B8" s="12" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C8" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="F8" s="18" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="I8" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="K8" s="18" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="N8" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C9" s="5">
         <v>0.63</v>
       </c>
       <c r="F9" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="I9" s="5">
         <v>0.03</v>
       </c>
       <c r="K9" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="N9" s="5">
         <v>0.01</v>
       </c>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C10" s="5">
         <v>0.37</v>
       </c>
       <c r="F10" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="I10" s="5">
         <v>0.02</v>
       </c>
       <c r="K10" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="N10" s="5">
         <v>0.03</v>
       </c>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F11" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="I11" s="5">
         <v>0.21</v>
       </c>
       <c r="K11" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="N11" s="5">
         <v>0.04</v>
       </c>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F12" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="I12" s="5">
         <v>0.5</v>
       </c>
       <c r="K12" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="N12" s="5">
         <v>0.11</v>
       </c>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F13" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="I13" s="5">
         <v>0.04</v>
       </c>
       <c r="K13" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="N13" s="19" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F14" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="I14" s="19" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="K14" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="N14">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F15" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="I15" s="5">
         <v>0.15</v>
       </c>
       <c r="K15" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="N15" s="5">
         <v>0.12</v>
       </c>
     </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F16" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="I16" s="5">
         <v>0.05</v>
       </c>
       <c r="K16" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="N16" s="5">
         <v>0.69</v>
       </c>
     </row>
-    <row r="18" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I18" s="5"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
edits to ensure flake8 passes and test files pass- one still not running
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_PregnancySupervisor.xlsx
+++ b/resources/ResourceFile_PregnancySupervisor.xlsx
@@ -9,16 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11670" windowHeight="6210" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11670" windowHeight="6210"/>
   </bookViews>
   <sheets>
     <sheet name="parameter_values" sheetId="1" r:id="rId1"/>
-    <sheet name="parameter_values_old" sheetId="7" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="6" r:id="rId3"/>
-    <sheet name="prob_pregnancy_factors" sheetId="2" r:id="rId4"/>
-    <sheet name="prob_maternal_death" sheetId="5" r:id="rId5"/>
-    <sheet name="md calculation" sheetId="3" r:id="rId6"/>
-    <sheet name="prob_stillbirth" sheetId="4" r:id="rId7"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId2"/>
+    <sheet name="prob_pregnancy_factors" sheetId="2" r:id="rId3"/>
+    <sheet name="prob_maternal_death" sheetId="5" r:id="rId4"/>
+    <sheet name="md calculation" sheetId="3" r:id="rId5"/>
+    <sheet name="prob_stillbirth" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -64,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="103">
   <si>
     <t>parameter_name</t>
   </si>
@@ -367,6 +366,12 @@
   </si>
   <si>
     <t>prob_induced_abortion_death</t>
+  </si>
+  <si>
+    <t>prob_ectopic_pregnancy_death</t>
+  </si>
+  <si>
+    <t>\</t>
   </si>
 </sst>
 </file>
@@ -776,10 +781,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -903,21 +908,18 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B11">
-        <v>0.05</v>
-      </c>
-      <c r="D11" t="s">
-        <v>19</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>94</v>
-      </c>
-      <c r="B12" t="s">
-        <v>97</v>
+        <v>100</v>
+      </c>
+      <c r="B12">
+        <v>0.05</v>
       </c>
       <c r="D12" t="s">
         <v>19</v>
@@ -925,10 +927,10 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D13" t="s">
         <v>19</v>
@@ -936,13 +938,29 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D14" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>96</v>
+      </c>
+      <c r="B15" t="s">
+        <v>99</v>
+      </c>
+      <c r="D15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K19" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -952,20 +970,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E18"/>
   <sheetViews>
@@ -1166,7 +1170,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G16"/>
   <sheetViews>
@@ -1449,7 +1453,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
@@ -1537,7 +1541,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O23"/>
   <sheetViews>
@@ -1830,7 +1834,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N18"/>
   <sheetViews>

</xml_diff>

<commit_message>
Labour May 2020 (#151)
* updates to newborn complications

* parameters now reading from resource file

* first iteration of antenatal care

* first iteration of hypertensive disorders of pregnancy module

* first iteration of pregnancy supervisor module

* Updates to HSI's to reflect recent version changes

Co-authored-by: Tim Hallett <timothy.hallett@imperial.ac.uk>
Co-authored-by: Stefan Piatek <s.piatek@ucl.ac.uk>
Co-authored-by: Asif Tamuri <tamuri@gmail.com>
Co-authored-by: Tim Hallett <tbhallett@gmail.com>
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_PregnancySupervisor.xlsx
+++ b/resources/ResourceFile_PregnancySupervisor.xlsx
@@ -9,14 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11676" windowHeight="6216" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11670" windowHeight="6210"/>
   </bookViews>
   <sheets>
     <sheet name="parameter_values" sheetId="1" r:id="rId1"/>
-    <sheet name="prob_pregnancy_factors" sheetId="2" r:id="rId2"/>
-    <sheet name="prob_maternal_death" sheetId="5" r:id="rId3"/>
-    <sheet name="md calculation" sheetId="3" r:id="rId4"/>
-    <sheet name="prob_stillbirth" sheetId="4" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId2"/>
+    <sheet name="prob_pregnancy_factors" sheetId="2" r:id="rId3"/>
+    <sheet name="prob_maternal_death" sheetId="5" r:id="rId4"/>
+    <sheet name="md calculation" sheetId="3" r:id="rId5"/>
+    <sheet name="prob_stillbirth" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -62,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="105">
   <si>
     <t>parameter_name</t>
   </si>
@@ -142,37 +143,6 @@
     <t>rr_gest_diab_chron_htn</t>
   </si>
   <si>
-    <t>base_prev_pe</t>
-  </si>
-  <si>
-    <t>base_prev_gest_htn</t>
-  </si>
-  <si>
-    <t>Pre-eclampsia, eclampsia and adverse maternal and perinatal outcomes: a secondary analysis of the World Health Organization Multicountry Survey on Maternal and Newborn Health.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#DUMMY </t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve"># partially dummy informed by </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Gestational diabetes mellitus in sub-Saharan Africa: Systematic review and metaregression on prevalence and risk factors</t>
-    </r>
-  </si>
-  <si>
-    <t>base_prev_gest_diab</t>
-  </si>
-  <si>
     <t>r_severe_pe_mild_pe</t>
   </si>
   <si>
@@ -354,6 +324,60 @@
   </si>
   <si>
     <t>risk_d_ectopic</t>
+  </si>
+  <si>
+    <t>prob_pre_eclampsia_per_month</t>
+  </si>
+  <si>
+    <t>prob_gest_htn_per_month</t>
+  </si>
+  <si>
+    <t>prob_gest_diab_per_month</t>
+  </si>
+  <si>
+    <t>prob_still_birth_per_month</t>
+  </si>
+  <si>
+    <t>prob_antenatal_death_per_month</t>
+  </si>
+  <si>
+    <t>[0.6, 0.4]</t>
+  </si>
+  <si>
+    <t>prob_induced_abortion_death</t>
+  </si>
+  <si>
+    <t>prob_ectopic_pregnancy_death</t>
+  </si>
+  <si>
+    <t>prob_spontaneous_abortion_per_month</t>
+  </si>
+  <si>
+    <t>prob_induced_abortion_per_month</t>
+  </si>
+  <si>
+    <t>prob_induced_abortion_type</t>
+  </si>
+  <si>
+    <t>prob_spontaneous_abortion_death</t>
+  </si>
+  <si>
+    <t>prob_haemorrhage_spontaneous_abortion</t>
+  </si>
+  <si>
+    <t>prob_sepsis_spontaneous_abortion</t>
+  </si>
+  <si>
+    <t>prob_haemorrhage_induced_abortion</t>
+  </si>
+  <si>
+    <t>prob_sepsis_induced_abortion</t>
+  </si>
+  <si>
+    <t>prob_injury_induced_abortion</t>
+  </si>
+  <si>
+    <t>prob_anaemia_per_month</t>
   </si>
 </sst>
 </file>
@@ -763,19 +787,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -786,245 +810,198 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="B2">
-        <v>2.1600000000000001E-2</v>
+        <v>0.02</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="B3">
         <v>0.02</v>
       </c>
-      <c r="E3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>95</v>
       </c>
       <c r="B4">
+        <v>0.02</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B5">
+        <v>0.02</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B6">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B7">
+        <v>0.02</v>
+      </c>
+      <c r="D7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>88</v>
+      </c>
+      <c r="B8">
+        <v>0.5</v>
+      </c>
+      <c r="C8">
+        <v>0.02</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>89</v>
+      </c>
+      <c r="B9">
+        <v>0.02</v>
+      </c>
+      <c r="D9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>90</v>
+      </c>
+      <c r="B10">
+        <v>0.02</v>
+      </c>
+      <c r="D10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>91</v>
+      </c>
+      <c r="B11">
+        <v>0.02</v>
+      </c>
+      <c r="D11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>94</v>
+      </c>
+      <c r="B12">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B13">
         <v>0.05</v>
       </c>
-      <c r="E4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5">
-        <v>2.23</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6">
-        <v>4.0199999999999996</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7">
-        <v>2.13</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8">
-        <v>0.49</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9">
-        <v>2.91</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10">
-        <v>7.19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11">
-        <v>3.51</v>
-      </c>
-      <c r="D11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12">
-        <v>2.92</v>
-      </c>
-      <c r="D12" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13">
-        <v>14.6</v>
-      </c>
       <c r="D13" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14">
-        <v>2.4900000000000002</v>
+        <v>97</v>
+      </c>
+      <c r="B14" t="s">
+        <v>92</v>
       </c>
       <c r="D14" t="s">
-        <v>21</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>99</v>
       </c>
       <c r="B15">
-        <v>0.02</v>
-      </c>
-      <c r="D15" t="s">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>100</v>
+      </c>
+      <c r="B16">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>101</v>
+      </c>
+      <c r="B17">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>102</v>
+      </c>
+      <c r="B18">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>103</v>
+      </c>
+      <c r="B19">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>98</v>
+      </c>
+      <c r="B20">
+        <v>0.05</v>
+      </c>
+      <c r="D20" t="s">
         <v>19</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16">
-        <v>0.02</v>
-      </c>
-      <c r="D16" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>40</v>
-      </c>
-      <c r="B17">
-        <v>0.6</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>35</v>
-      </c>
-      <c r="B18">
-        <v>3.4000000000000002E-2</v>
-      </c>
-      <c r="D18" t="s">
-        <v>36</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>32</v>
-      </c>
-      <c r="B19">
-        <v>3.4000000000000002E-2</v>
-      </c>
-      <c r="D19" t="s">
-        <v>36</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>33</v>
-      </c>
-      <c r="B20">
-        <v>3.4000000000000002E-2</v>
-      </c>
-      <c r="D20" t="s">
-        <v>36</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>34</v>
-      </c>
-      <c r="B21">
-        <v>3.4000000000000002E-2</v>
-      </c>
-      <c r="D21" t="s">
-        <v>36</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1035,23 +1012,224 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:E18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2">
+        <v>2.23</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3">
+        <v>4.0199999999999996</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>2.13</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>0.49</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6">
+        <v>2.91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7">
+        <v>7.19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8">
+        <v>3.51</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9">
+        <v>2.92</v>
+      </c>
+      <c r="D9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10">
+        <v>14.6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11">
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="D11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14">
+        <v>0.6</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="D16" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="D17" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="D18" t="s">
+        <v>30</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1074,7 +1252,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1097,7 +1275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1120,7 +1298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1143,7 +1321,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1166,7 +1344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1189,7 +1367,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1212,7 +1390,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1235,7 +1413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1258,7 +1436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1281,7 +1459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1304,7 +1482,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16">
         <f>SUM(B2:B6)</f>
         <v>0.19</v>
@@ -1316,85 +1494,85 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C1" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D1" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="E1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1404,7 +1582,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O23"/>
   <sheetViews>
@@ -1412,24 +1590,24 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="24.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.77734375" customWidth="1"/>
-    <col min="4" max="4" width="12.88671875" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
     <col min="8" max="8" width="11" customWidth="1"/>
     <col min="10" max="10" width="17" customWidth="1"/>
-    <col min="15" max="15" width="25.33203125" customWidth="1"/>
+    <col min="15" max="15" width="25.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B1" s="16" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C4" s="4">
         <v>2010</v>
@@ -1462,72 +1640,72 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C5">
         <v>484</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="H5">
         <v>451</v>
       </c>
       <c r="I5" s="11" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="J5" s="11" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="K5" s="11" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="L5" s="11" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C6" s="6" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="H6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="9" spans="2:15" ht="43.2" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" ht="60" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D9" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="J9" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="H9" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="I9" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="J9" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C10" s="5">
         <v>0.3</v>
@@ -1536,15 +1714,15 @@
         <v>0.22700000000000001</v>
       </c>
       <c r="H10" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="I10" s="10">
         <v>9.6000000000000002E-2</v>
       </c>
     </row>
-    <row r="11" spans="2:15" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:15" ht="45" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C11" s="5">
         <v>0.4</v>
@@ -1553,21 +1731,21 @@
         <v>0.48599999999999999</v>
       </c>
       <c r="H11" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="I11" s="10">
         <v>2.1000000000000001E-2</v>
       </c>
       <c r="K11" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="O11" s="7" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C12" s="5">
         <v>0.3</v>
@@ -1576,73 +1754,73 @@
         <v>0.28699999999999998</v>
       </c>
       <c r="H12" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="I12" s="10">
         <v>0.245</v>
       </c>
     </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H13" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="I13" s="5">
         <v>0.16</v>
       </c>
     </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C14" s="5">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="H14" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="I14" s="10">
         <v>0.10299999999999999</v>
       </c>
     </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C15" s="5">
         <v>0.08</v>
       </c>
       <c r="H15" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="I15" s="5">
         <v>0.09</v>
       </c>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C16" s="5">
         <v>0.15</v>
       </c>
       <c r="H16" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="I16" s="10">
         <v>0.28599999999999998</v>
       </c>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C17" s="5">
         <v>0.4</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C18" s="5">
         <v>0.09</v>
@@ -1652,39 +1830,39 @@
         <v>1.0009999999999999</v>
       </c>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C19" s="5">
         <v>0.21</v>
       </c>
     </row>
-    <row r="21" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:11" ht="45" x14ac:dyDescent="0.25">
       <c r="H21" s="13" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="I21" s="14" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="J21" s="15"/>
       <c r="K21" s="15"/>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
       <c r="H22" s="15"/>
       <c r="I22" s="15" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="J22" s="15" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="K22" s="15" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
       <c r="H23" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="I23" s="5"/>
       <c r="J23" s="5">
@@ -1697,7 +1875,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N18"/>
   <sheetViews>
@@ -1705,20 +1883,20 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B1" s="16" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C4" s="17">
         <v>2010</v>
@@ -1751,164 +1929,164 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="H5">
         <v>21.8</v>
       </c>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="H6" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="8" spans="2:14" ht="28.8" x14ac:dyDescent="0.3">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" ht="30" x14ac:dyDescent="0.25">
       <c r="B8" s="12" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C8" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="F8" s="18" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="I8" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="K8" s="18" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="N8" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C9" s="5">
         <v>0.63</v>
       </c>
       <c r="F9" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="I9" s="5">
         <v>0.03</v>
       </c>
       <c r="K9" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="N9" s="5">
         <v>0.01</v>
       </c>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C10" s="5">
         <v>0.37</v>
       </c>
       <c r="F10" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="I10" s="5">
         <v>0.02</v>
       </c>
       <c r="K10" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="N10" s="5">
         <v>0.03</v>
       </c>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F11" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="I11" s="5">
         <v>0.21</v>
       </c>
       <c r="K11" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="N11" s="5">
         <v>0.04</v>
       </c>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F12" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="I12" s="5">
         <v>0.5</v>
       </c>
       <c r="K12" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="N12" s="5">
         <v>0.11</v>
       </c>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F13" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="I13" s="5">
         <v>0.04</v>
       </c>
       <c r="K13" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="N13" s="19" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F14" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="I14" s="19" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="K14" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="N14">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F15" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="I15" s="5">
         <v>0.15</v>
       </c>
       <c r="K15" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="N15" s="5">
         <v>0.12</v>
       </c>
     </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
       <c r="F16" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="I16" s="5">
         <v>0.05</v>
       </c>
       <c r="K16" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="N16" s="5">
         <v>0.69</v>
       </c>
     </row>
-    <row r="18" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I18" s="5"/>
     </row>
   </sheetData>

</xml_diff>